<commit_message>
commit all code 27/11
</commit_message>
<xml_diff>
--- a/Excel TC/SampleProject_TC_Text.xlsx
+++ b/Excel TC/SampleProject_TC_Text.xlsx
@@ -1137,9 +1137,6 @@
   </si>
   <si>
     <t>Verify Equal</t>
-  </si>
-  <si>
-    <t>Select Description from Static_Content Where Type_Testing = "text"</t>
   </si>
   <si>
     <t>Send Request</t>
@@ -1370,6 +1367,9 @@
   </si>
   <si>
     <t>0.0</t>
+  </si>
+  <si>
+    <t>Select Description from Static_Content  Where Type_Testing = 'text'</t>
   </si>
 </sst>
 </file>
@@ -2325,6 +2325,9 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2357,9 +2360,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="361">
@@ -3026,7 +3026,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>
@@ -3078,7 +3078,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>
@@ -3130,7 +3130,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>
@@ -3507,18 +3507,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="23.1" customHeight="1">
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="C3" s="55"/>
+      <c r="C3" s="56"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="C4" s="55"/>
+      <c r="C4" s="56"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="C5" s="55"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="2:11" ht="26.1" customHeight="1"/>
     <row r="7" spans="2:11" ht="15.75">
@@ -3642,18 +3642,18 @@
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="2:11" ht="15">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
     </row>
     <row r="17" spans="2:11" ht="15">
       <c r="B17" s="21" t="s">
@@ -3736,14 +3736,14 @@
       <c r="K21" s="6"/>
     </row>
     <row r="23" spans="2:11" ht="15">
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="8" t="s">
@@ -3802,10 +3802,10 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3970,7 +3970,7 @@
         <v>302</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L3" s="39" t="s">
         <v>54</v>
@@ -4061,7 +4061,7 @@
         <v>303</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L5" s="39" t="s">
         <v>54</v>
@@ -4144,12 +4144,12 @@
         <v>304</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
       <c r="N7" s="39" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="O7" s="48" t="s">
         <v>61</v>
@@ -4232,19 +4232,19 @@
         <v>67</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L9" s="39" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M9" s="39" t="s">
         <v>54</v>
       </c>
       <c r="N9" s="39" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O9" s="39"/>
       <c r="P9" s="39"/>
@@ -4287,18 +4287,18 @@
         <v>66</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>308</v>
-      </c>
-      <c r="K10" s="59" t="s">
-        <v>327</v>
+        <v>307</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>326</v>
       </c>
       <c r="L10" s="39"/>
       <c r="M10" s="39"/>
       <c r="N10" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="O10" s="39" t="s">
         <v>309</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>310</v>
       </c>
       <c r="P10" s="39"/>
       <c r="Q10" s="39"/>
@@ -4322,16 +4322,16 @@
       <c r="H11" s="44"/>
       <c r="I11" s="39"/>
       <c r="J11" s="48" t="s">
-        <v>308</v>
-      </c>
-      <c r="K11" s="60"/>
+        <v>307</v>
+      </c>
+      <c r="K11" s="61"/>
       <c r="L11" s="39"/>
       <c r="M11" s="39"/>
       <c r="N11" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="O11" s="39" t="s">
         <v>312</v>
-      </c>
-      <c r="O11" s="39" t="s">
-        <v>313</v>
       </c>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
@@ -4355,16 +4355,16 @@
       <c r="H12" s="53"/>
       <c r="I12" s="51"/>
       <c r="J12" s="48" t="s">
-        <v>308</v>
-      </c>
-      <c r="K12" s="60"/>
+        <v>307</v>
+      </c>
+      <c r="K12" s="61"/>
       <c r="L12" s="51"/>
       <c r="M12" s="51"/>
       <c r="N12" s="51" t="s">
+        <v>313</v>
+      </c>
+      <c r="O12" s="51" t="s">
         <v>314</v>
-      </c>
-      <c r="O12" s="51" t="s">
-        <v>315</v>
       </c>
       <c r="P12" s="51"/>
       <c r="Q12" s="51"/>
@@ -4388,13 +4388,13 @@
       <c r="H13" s="53"/>
       <c r="I13" s="51"/>
       <c r="J13" s="48" t="s">
-        <v>308</v>
-      </c>
-      <c r="K13" s="61"/>
+        <v>307</v>
+      </c>
+      <c r="K13" s="62"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51"/>
       <c r="N13" s="51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O13" s="51">
         <v>50667</v>
@@ -4469,19 +4469,19 @@
         <v>67</v>
       </c>
       <c r="J15" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>327</v>
+      </c>
+      <c r="L15" s="39" t="s">
         <v>306</v>
-      </c>
-      <c r="K15" s="48" t="s">
-        <v>328</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>307</v>
       </c>
       <c r="M15" s="39" t="s">
         <v>54</v>
       </c>
       <c r="N15" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O15" s="39" t="s">
         <v>75</v>
@@ -4532,18 +4532,18 @@
         <v>74</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>318</v>
-      </c>
-      <c r="K16" s="59" t="s">
-        <v>327</v>
+        <v>317</v>
+      </c>
+      <c r="K16" s="60" t="s">
+        <v>326</v>
       </c>
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
       <c r="N16" s="39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O16" s="39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P16" s="39"/>
       <c r="Q16" s="39"/>
@@ -4567,16 +4567,16 @@
       <c r="H17" s="53"/>
       <c r="I17" s="51"/>
       <c r="J17" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="K17" s="60"/>
+        <v>317</v>
+      </c>
+      <c r="K17" s="61"/>
       <c r="L17" s="51"/>
       <c r="M17" s="51"/>
       <c r="N17" s="51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O17" s="51" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P17" s="51"/>
       <c r="Q17" s="51"/>
@@ -4600,13 +4600,13 @@
       <c r="H18" s="53"/>
       <c r="I18" s="51"/>
       <c r="J18" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="K18" s="60"/>
+        <v>317</v>
+      </c>
+      <c r="K18" s="61"/>
       <c r="L18" s="51"/>
       <c r="M18" s="51"/>
       <c r="N18" s="51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O18" s="51">
         <v>407</v>
@@ -4633,13 +4633,13 @@
       <c r="H19" s="53"/>
       <c r="I19" s="51"/>
       <c r="J19" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="K19" s="60"/>
+        <v>317</v>
+      </c>
+      <c r="K19" s="61"/>
       <c r="L19" s="51"/>
       <c r="M19" s="51"/>
       <c r="N19" s="51" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O19" s="51">
         <v>143</v>
@@ -4666,13 +4666,13 @@
       <c r="H20" s="53"/>
       <c r="I20" s="51"/>
       <c r="J20" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="K20" s="60"/>
+        <v>317</v>
+      </c>
+      <c r="K20" s="61"/>
       <c r="L20" s="51"/>
       <c r="M20" s="51"/>
       <c r="N20" s="51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O20" s="51">
         <v>143</v>
@@ -4699,16 +4699,16 @@
       <c r="H21" s="53"/>
       <c r="I21" s="51"/>
       <c r="J21" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="K21" s="61"/>
+        <v>317</v>
+      </c>
+      <c r="K21" s="62"/>
       <c r="L21" s="51"/>
       <c r="M21" s="51"/>
       <c r="N21" s="51" t="s">
-        <v>324</v>
-      </c>
-      <c r="O21" s="66" t="s">
-        <v>332</v>
+        <v>323</v>
+      </c>
+      <c r="O21" s="55" t="s">
+        <v>331</v>
       </c>
       <c r="P21" s="51"/>
       <c r="Q21" s="51"/>
@@ -4944,12 +4944,12 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
       <c r="A3" s="25"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="37" t="s">
         <v>84</v>
       </c>
@@ -4960,10 +4960,10 @@
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
@@ -4972,10 +4972,10 @@
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1">
       <c r="A5" s="25"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -4996,12 +4996,12 @@
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
       <c r="A7" s="25"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="37" t="s">
@@ -5014,12 +5014,12 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="31"/>

</xml_diff>

<commit_message>
Commit all code to branch
</commit_message>
<xml_diff>
--- a/Excel TC/SampleProject_TC_Text.xlsx
+++ b/Excel TC/SampleProject_TC_Text.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="14805" windowHeight="8010" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="14805" windowHeight="7695" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -3026,7 +3026,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>
@@ -3078,7 +3078,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>
@@ -3130,7 +3130,7 @@
         <xdr:cNvSpPr>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_14_oaTxWxMAAAAlAAAAZAAAAIwAAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAEAAAAAAAAA///hAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAABAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAQAAAAAAAAAEAAAAAAAAAAEAAAAAAAAAAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAy8vLAAAAAAAoAAAAKAAAAGQAAABkAAAAAAAAABcAAAAUAAAAAAAAAAAAAAD/fwAA/38AAAAAAAAJAAAABAAAAAAAAAAMAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAECcAABAnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQAAAAAAAAAwMD/AAAAAABkAAAAMgAAAAAAAABkAAAAAAAAAH9/fwAKAAAAIgAAABgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAkAAAAJAAAAAAAAAAHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf39/ACUAAABYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/AAAAAAAAAKCGAQAAAAAAAAAAAAAAAAAMAAAAAQAAAAAAAAAAAAAAAAAAACEAAAAwAAAALAAAAAEAAAABAAAAZgFRAAMAAAAFAAAADwNpADEIAACVAQAA4RYAALICAAACAAAA"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvSpPr>

</xml_diff>